<commit_message>
Fix waste index report
</commit_message>
<xml_diff>
--- a/storage/templates/waste-index.xlsx
+++ b/storage/templates/waste-index.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/apps/cost-control/storage/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/code/cost-control/storage/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1C90E0-6ABB-7744-84EA-657A5CBC3CF9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Material Consumption Index" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -83,8 +84,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,6 +128,7 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -134,6 +136,14 @@
       <sz val="12"/>
       <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -171,36 +181,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="40" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="40" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -477,24 +490,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="62.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="25" style="8" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="8" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="22" style="8" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
     <col min="10" max="10" width="19.5" customWidth="1"/>
     <col min="11" max="11" width="20.33203125" customWidth="1"/>
     <col min="12" max="12" width="33.5" customWidth="1"/>
@@ -502,162 +515,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="B8"/>
-      <c r="C8" s="5" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2">
         <v>0</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="2">
         <v>0</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="2">
         <v>0</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix material waste index label in reports
</commit_message>
<xml_diff>
--- a/storage/templates/waste-index.xlsx
+++ b/storage/templates/waste-index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/code/cost-control/storage/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1C90E0-6ABB-7744-84EA-657A5CBC3CF9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFCEF69-0E0B-D44F-833E-8BB14C325DC5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Period:</t>
   </si>
   <si>
-    <t>Waste Index</t>
-  </si>
-  <si>
     <t>To Date Unit Price</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Material Consumption Index</t>
   </si>
 </sst>
 </file>
@@ -203,11 +203,11 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -494,7 +494,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,12 +606,12 @@
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="C8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -632,33 +632,33 @@
         <v>0</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -673,7 +673,7 @@
       <c r="H11" s="2">
         <v>0</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <v>0</v>
       </c>
     </row>

</xml_diff>